<commit_message>
remove legacy data for consistency
</commit_message>
<xml_diff>
--- a/results/aggregated/result_androzoo_basic_dnn.xlsx
+++ b/results/aggregated/result_androzoo_basic_dnn.xlsx
@@ -749,13 +749,13 @@
         <v>59.8828125</v>
       </c>
       <c r="C5">
-        <v>58.80078256130219</v>
+        <v>58.50000262260437</v>
       </c>
       <c r="D5">
         <v>59.8828125</v>
       </c>
       <c r="E5">
-        <v>59.38672006130219</v>
+        <v>58.50000262260437</v>
       </c>
       <c r="F5">
         <v>59.8828125</v>
@@ -773,13 +773,13 @@
         <v>59.8828125</v>
       </c>
       <c r="K5">
-        <v>58.67578268051147</v>
+        <v>58.25000286102295</v>
       </c>
       <c r="L5">
         <v>59.8828125</v>
       </c>
       <c r="M5">
-        <v>59.14843857288361</v>
+        <v>59.00000214576721</v>
       </c>
       <c r="N5">
         <v>59.8828125</v>
@@ -797,13 +797,13 @@
         <v>0.703125</v>
       </c>
       <c r="S5">
-        <v>2.945313155651093</v>
+        <v>0.5000013113021851</v>
       </c>
       <c r="T5">
         <v>0.703125</v>
       </c>
       <c r="U5">
-        <v>0.6015631556510925</v>
+        <v>0.5000013113021851</v>
       </c>
       <c r="V5">
         <v>59.8828125</v>
@@ -821,13 +821,13 @@
         <v>0.703125</v>
       </c>
       <c r="AA5">
-        <v>2.945313155651093</v>
+        <v>0.5000013113021851</v>
       </c>
       <c r="AB5">
         <v>0.703125</v>
       </c>
       <c r="AC5">
-        <v>0.6015631556510925</v>
+        <v>0.5000013113021851</v>
       </c>
       <c r="AD5">
         <v>59.8828125</v>
@@ -845,7 +845,7 @@
         <v>59.8828125</v>
       </c>
       <c r="AI5">
-        <v>58.77343893051147</v>
+        <v>58.25000286102295</v>
       </c>
       <c r="AJ5">
         <v>59.8828125</v>
@@ -880,13 +880,13 @@
         <v>55.3828125</v>
       </c>
       <c r="C6">
-        <v>54.07812643051147</v>
+        <v>53.75000286102295</v>
       </c>
       <c r="D6">
         <v>55.3828125</v>
       </c>
       <c r="E6">
-        <v>54.44140481948853</v>
+        <v>53.49999713897705</v>
       </c>
       <c r="F6">
         <v>55.3828125</v>
@@ -904,13 +904,13 @@
         <v>55.3828125</v>
       </c>
       <c r="K6">
-        <v>53.20312428474426</v>
+        <v>51.99999856948853</v>
       </c>
       <c r="L6">
         <v>55.3828125</v>
       </c>
       <c r="M6">
-        <v>54.07812643051147</v>
+        <v>53.75000286102295</v>
       </c>
       <c r="N6">
         <v>55.3828125</v>
@@ -928,13 +928,13 @@
         <v>1.0859375</v>
       </c>
       <c r="S6">
-        <v>1.4765625</v>
+        <v>0.5</v>
       </c>
       <c r="T6">
         <v>1.0859375</v>
       </c>
       <c r="U6">
-        <v>0.890625</v>
+        <v>0.5</v>
       </c>
       <c r="V6">
         <v>55.3828125</v>
@@ -952,13 +952,13 @@
         <v>1.0859375</v>
       </c>
       <c r="AA6">
-        <v>1.4765625</v>
+        <v>0.5</v>
       </c>
       <c r="AB6">
         <v>1.0859375</v>
       </c>
       <c r="AC6">
-        <v>0.890625</v>
+        <v>0.5</v>
       </c>
       <c r="AD6">
         <v>2.453125</v>
@@ -976,7 +976,7 @@
         <v>55.3828125</v>
       </c>
       <c r="AI6">
-        <v>54.37109518051147</v>
+        <v>53.75000286102295</v>
       </c>
       <c r="AJ6">
         <v>55.3828125</v>
@@ -1011,13 +1011,13 @@
         <v>50.2421875</v>
       </c>
       <c r="C7">
-        <v>49.23047018051147</v>
+        <v>49.00000286102295</v>
       </c>
       <c r="D7">
         <v>50.2421875</v>
       </c>
       <c r="E7">
-        <v>49.07812368869781</v>
+        <v>48.49999737739563</v>
       </c>
       <c r="F7">
         <v>50.2421875</v>
@@ -1035,13 +1035,13 @@
         <v>50.2421875</v>
       </c>
       <c r="K7">
-        <v>49.20312356948853</v>
+        <v>48.74999713897705</v>
       </c>
       <c r="L7">
         <v>50.2421875</v>
       </c>
       <c r="M7">
-        <v>49.07812368869781</v>
+        <v>48.49999737739563</v>
       </c>
       <c r="N7">
         <v>50.2421875</v>
@@ -1059,13 +1059,13 @@
         <v>1.0234375</v>
       </c>
       <c r="S7">
-        <v>2.031250715255737</v>
+        <v>0.5000014305114746</v>
       </c>
       <c r="T7">
         <v>1.0234375</v>
       </c>
       <c r="U7">
-        <v>2.031250715255737</v>
+        <v>0.5000014305114746</v>
       </c>
       <c r="V7">
         <v>1.21875</v>
@@ -1083,13 +1083,13 @@
         <v>1.0234375</v>
       </c>
       <c r="AA7">
-        <v>2.031250715255737</v>
+        <v>0.5000014305114746</v>
       </c>
       <c r="AB7">
         <v>1.0234375</v>
       </c>
       <c r="AC7">
-        <v>2.031250715255737</v>
+        <v>0.5000014305114746</v>
       </c>
       <c r="AD7">
         <v>1.21875</v>
@@ -1107,7 +1107,7 @@
         <v>50.2421875</v>
       </c>
       <c r="AI7">
-        <v>49.10546731948853</v>
+        <v>48.74999713897705</v>
       </c>
       <c r="AJ7">
         <v>50.2421875</v>
@@ -1142,13 +1142,13 @@
         <v>43.9921875</v>
       </c>
       <c r="C8">
-        <v>42.67578017711639</v>
+        <v>41.74999785423279</v>
       </c>
       <c r="D8">
         <v>43.9921875</v>
       </c>
       <c r="E8">
-        <v>43.4257824420929</v>
+        <v>43.25000238418579</v>
       </c>
       <c r="F8">
         <v>43.9921875</v>
@@ -1166,13 +1166,13 @@
         <v>43.9921875</v>
       </c>
       <c r="K8">
-        <v>41.52343761920929</v>
+        <v>39.25000023841858</v>
       </c>
       <c r="L8">
         <v>43.9921875</v>
       </c>
       <c r="M8">
-        <v>43.30078256130219</v>
+        <v>43.00000262260437</v>
       </c>
       <c r="N8">
         <v>43.9921875</v>
@@ -1190,13 +1190,13 @@
         <v>0.2421875</v>
       </c>
       <c r="S8">
-        <v>1.781250953674316</v>
+        <v>1.9073486328125E-06</v>
       </c>
       <c r="T8">
         <v>0.2421875</v>
       </c>
       <c r="U8">
-        <v>0.2187509536743164</v>
+        <v>1.9073486328125E-06</v>
       </c>
       <c r="V8">
         <v>0.4375</v>
@@ -1214,13 +1214,13 @@
         <v>0.2421875</v>
       </c>
       <c r="AA8">
-        <v>1.781250953674316</v>
+        <v>1.9073486328125E-06</v>
       </c>
       <c r="AB8">
         <v>0.2421875</v>
       </c>
       <c r="AC8">
-        <v>0.2187509536743164</v>
+        <v>1.9073486328125E-06</v>
       </c>
       <c r="AD8">
         <v>0.4375</v>
@@ -1238,7 +1238,7 @@
         <v>43.9921875</v>
       </c>
       <c r="AI8">
-        <v>42.42578041553497</v>
+        <v>41.24999833106995</v>
       </c>
       <c r="AJ8">
         <v>43.9921875</v>
@@ -1273,13 +1273,13 @@
         <v>37.18749999999999</v>
       </c>
       <c r="C9">
-        <v>36.39843881130218</v>
+        <v>36.00000262260436</v>
       </c>
       <c r="D9">
         <v>37.38281249999999</v>
       </c>
       <c r="E9">
-        <v>36.30078256130218</v>
+        <v>36.00000262260436</v>
       </c>
       <c r="F9">
         <v>37.38281249999999</v>
@@ -1297,13 +1297,13 @@
         <v>37.38281249999999</v>
       </c>
       <c r="K9">
-        <v>36.10547006130218</v>
+        <v>36.00000262260436</v>
       </c>
       <c r="L9">
         <v>37.38281249999999</v>
       </c>
       <c r="M9">
-        <v>36.42578244209288</v>
+        <v>36.25000238418577</v>
       </c>
       <c r="N9">
         <v>37.38281249999999</v>
@@ -1321,13 +1321,13 @@
         <v>1.445312499999993</v>
       </c>
       <c r="S9">
-        <v>0.8476567268371512</v>
+        <v>0.2500009536743093</v>
       </c>
       <c r="T9">
         <v>1.445312499999993</v>
       </c>
       <c r="U9">
-        <v>0.7500004768371511</v>
+        <v>0.2500009536743093</v>
       </c>
       <c r="V9">
         <v>1.445312499999993</v>
@@ -1345,13 +1345,13 @@
         <v>1.445312499999993</v>
       </c>
       <c r="AA9">
-        <v>0.8476567268371512</v>
+        <v>0.2500009536743093</v>
       </c>
       <c r="AB9">
         <v>1.445312499999993</v>
       </c>
       <c r="AC9">
-        <v>0.7500004768371511</v>
+        <v>0.2500009536743093</v>
       </c>
       <c r="AD9">
         <v>1.445312499999993</v>
@@ -1369,7 +1369,7 @@
         <v>37.38281249999999</v>
       </c>
       <c r="AI9">
-        <v>34.41797018051147</v>
+        <v>35.75000286102294</v>
       </c>
       <c r="AJ9">
         <v>37.38281249999999</v>
@@ -1404,13 +1404,13 @@
         <v>31.6875</v>
       </c>
       <c r="C10">
-        <v>26.80078041553497</v>
+        <v>22.49999833106995</v>
       </c>
       <c r="D10">
         <v>31.6875</v>
       </c>
       <c r="E10">
-        <v>30.14843654632568</v>
+        <v>28.99999809265137</v>
       </c>
       <c r="F10">
         <v>31.6875</v>
@@ -1428,13 +1428,13 @@
         <v>14.6953125</v>
       </c>
       <c r="K10">
-        <v>9.960936427116394</v>
+        <v>10.49999785423279</v>
       </c>
       <c r="L10">
         <v>31.6875</v>
       </c>
       <c r="M10">
-        <v>30.57812643051147</v>
+        <v>30.25000286102295</v>
       </c>
       <c r="N10">
         <v>31.6875</v>
@@ -1452,13 +1452,13 @@
         <v>1.21875</v>
       </c>
       <c r="S10">
-        <v>0.6367195844650269</v>
+        <v>0.2500016689300537</v>
       </c>
       <c r="T10">
         <v>1.21875</v>
       </c>
       <c r="U10">
-        <v>0.5390633344650269</v>
+        <v>0.2500016689300537</v>
       </c>
       <c r="V10">
         <v>1.21875</v>
@@ -1476,13 +1476,13 @@
         <v>1.21875</v>
       </c>
       <c r="AA10">
-        <v>0.6367195844650269</v>
+        <v>0.2500016689300537</v>
       </c>
       <c r="AB10">
         <v>1.21875</v>
       </c>
       <c r="AC10">
-        <v>0.5390633344650269</v>
+        <v>0.2500016689300537</v>
       </c>
       <c r="AD10">
         <v>1.21875</v>
@@ -1500,7 +1500,7 @@
         <v>31.6875</v>
       </c>
       <c r="AI10">
-        <v>30.77343893051147</v>
+        <v>30.25000286102295</v>
       </c>
       <c r="AJ10">
         <v>31.6875</v>
@@ -1535,13 +1535,13 @@
         <v>25.6875</v>
       </c>
       <c r="C11">
-        <v>15.6484386920929</v>
+        <v>6.000002384185791</v>
       </c>
       <c r="D11">
         <v>25.6875</v>
       </c>
       <c r="E11">
-        <v>22.82812511920929</v>
+        <v>20.75000023841858</v>
       </c>
       <c r="F11">
         <v>25.6875</v>
@@ -1559,13 +1559,13 @@
         <v>25.4921875</v>
       </c>
       <c r="K11">
-        <v>24.42577993869781</v>
+        <v>23.74999737739563</v>
       </c>
       <c r="L11">
         <v>25.6875</v>
       </c>
       <c r="M11">
-        <v>25.0234386920929</v>
+        <v>24.75000238418579</v>
       </c>
       <c r="N11">
         <v>25.6875</v>
@@ -1583,13 +1583,13 @@
         <v>0.4921875</v>
       </c>
       <c r="S11">
-        <v>0.4960945844650269</v>
+        <v>0.5000016689300537</v>
       </c>
       <c r="T11">
         <v>0.4921875</v>
       </c>
       <c r="U11">
-        <v>0.3984383344650269</v>
+        <v>0.5000016689300537</v>
       </c>
       <c r="V11">
         <v>0.6875</v>
@@ -1607,13 +1607,13 @@
         <v>0.4921875</v>
       </c>
       <c r="AA11">
-        <v>0.4960945844650269</v>
+        <v>0.5000016689300537</v>
       </c>
       <c r="AB11">
         <v>0.4921875</v>
       </c>
       <c r="AC11">
-        <v>0.3984383344650269</v>
+        <v>0.5000016689300537</v>
       </c>
       <c r="AD11">
         <v>0.6875</v>
@@ -1631,7 +1631,7 @@
         <v>25.296875</v>
       </c>
       <c r="AI11">
-        <v>22.14453136920929</v>
+        <v>20.75000023841858</v>
       </c>
       <c r="AJ11">
         <v>25.4921875</v>
@@ -1666,13 +1666,13 @@
         <v>20.3828125</v>
       </c>
       <c r="C12">
-        <v>16.92578184604645</v>
+        <v>14.2500011920929</v>
       </c>
       <c r="D12">
         <v>20.3828125</v>
       </c>
       <c r="E12">
-        <v>19.4257824420929</v>
+        <v>19.25000238418579</v>
       </c>
       <c r="F12">
         <v>20.3828125</v>
@@ -1690,13 +1690,13 @@
         <v>19.015625</v>
       </c>
       <c r="K12">
-        <v>9.851562857627869</v>
+        <v>8.500000715255737</v>
       </c>
       <c r="L12">
         <v>20.3828125</v>
       </c>
       <c r="M12">
-        <v>18.62109291553497</v>
+        <v>17.24999833106995</v>
       </c>
       <c r="N12">
         <v>20.3828125</v>
@@ -1714,13 +1714,13 @@
         <v>1.2421875</v>
       </c>
       <c r="S12">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="T12">
         <v>1.2421875</v>
       </c>
       <c r="U12">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="V12">
         <v>1.2421875</v>
@@ -1738,13 +1738,13 @@
         <v>1.2421875</v>
       </c>
       <c r="AA12">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="AB12">
         <v>1.2421875</v>
       </c>
       <c r="AC12">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="AD12">
         <v>1.2421875</v>
@@ -1762,7 +1762,7 @@
         <v>19.2109375</v>
       </c>
       <c r="AI12">
-        <v>16.89843821525574</v>
+        <v>14.00000143051147</v>
       </c>
       <c r="AJ12">
         <v>20.3828125</v>
@@ -1797,13 +1797,13 @@
         <v>12.265625</v>
       </c>
       <c r="C13">
-        <v>5.671876072883606</v>
+        <v>0.2500021457672119</v>
       </c>
       <c r="D13">
         <v>14.0234375</v>
       </c>
       <c r="E13">
-        <v>11.39843702316284</v>
+        <v>9.749999046325684</v>
       </c>
       <c r="F13">
         <v>14.0234375</v>
@@ -1821,13 +1821,13 @@
         <v>13.828125</v>
       </c>
       <c r="K13">
-        <v>12.13281393051147</v>
+        <v>12.00000286102295</v>
       </c>
       <c r="L13">
         <v>14.0234375</v>
       </c>
       <c r="M13">
-        <v>12.74609506130219</v>
+        <v>12.25000262260437</v>
       </c>
       <c r="N13">
         <v>14.0234375</v>
@@ -1845,13 +1845,13 @@
         <v>0.7421875</v>
       </c>
       <c r="S13">
-        <v>0.8164072036743164</v>
+        <v>0.5000019073486328</v>
       </c>
       <c r="T13">
         <v>0.7421875</v>
       </c>
       <c r="U13">
-        <v>0.6210947036743164</v>
+        <v>0.5000019073486328</v>
       </c>
       <c r="V13">
         <v>0.7421875</v>
@@ -1869,13 +1869,13 @@
         <v>0.7421875</v>
       </c>
       <c r="AA13">
-        <v>0.8164072036743164</v>
+        <v>0.5000019073486328</v>
       </c>
       <c r="AB13">
         <v>0.7421875</v>
       </c>
       <c r="AC13">
-        <v>0.6210947036743164</v>
+        <v>0.5000019073486328</v>
       </c>
       <c r="AD13">
         <v>0.7421875</v>
@@ -1893,7 +1893,7 @@
         <v>13.6328125</v>
       </c>
       <c r="AI13">
-        <v>11.17578089237213</v>
+        <v>9.499999284744264</v>
       </c>
       <c r="AJ13">
         <v>14.0234375</v>
@@ -1928,13 +1928,13 @@
         <v>8.078125</v>
       </c>
       <c r="C14">
-        <v>5.46874988079071</v>
+        <v>3.249999761581421</v>
       </c>
       <c r="D14">
         <v>8.2734375</v>
       </c>
       <c r="E14">
-        <v>6.566405177116394</v>
+        <v>5.249997854232788</v>
       </c>
       <c r="F14">
         <v>8.2734375</v>
@@ -1952,13 +1952,13 @@
         <v>7.1015625</v>
       </c>
       <c r="K14">
-        <v>3.382813811302185</v>
+        <v>0.2500026226043701</v>
       </c>
       <c r="L14">
         <v>7.296875</v>
       </c>
       <c r="M14">
-        <v>4.312500238418579</v>
+        <v>2.500000476837158</v>
       </c>
       <c r="N14">
         <v>8.2734375</v>
@@ -1976,13 +1976,13 @@
         <v>1.046875</v>
       </c>
       <c r="S14">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="T14">
         <v>1.046875</v>
       </c>
       <c r="U14">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="V14">
         <v>1.046875</v>
@@ -2000,13 +2000,13 @@
         <v>1.046875</v>
       </c>
       <c r="AA14">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="AB14">
         <v>1.046875</v>
       </c>
       <c r="AC14">
-        <v>0.8710949420928955</v>
+        <v>0.500002384185791</v>
       </c>
       <c r="AD14">
         <v>1.046875</v>
@@ -2024,7 +2024,7 @@
         <v>8.2734375</v>
       </c>
       <c r="AI14">
-        <v>7.566407203674316</v>
+        <v>7.250001907348633</v>
       </c>
       <c r="AJ14">
         <v>8.2734375</v>
@@ -18457,6 +18457,9 @@
       <c r="AO37">
         <v>1.500001621246341</v>
       </c>
+      <c r="AP37">
+        <v>2.624997568130496</v>
+      </c>
       <c r="AQ37">
         <v>2.900001478195193</v>
       </c>
@@ -18585,6 +18588,9 @@
       <c r="AO38">
         <v>2.075000143051142</v>
       </c>
+      <c r="AP38">
+        <v>2.700000190734869</v>
+      </c>
       <c r="AQ38">
         <v>2.899999952316278</v>
       </c>
@@ -18713,6 +18719,9 @@
       <c r="AO39">
         <v>2.149998903274536</v>
       </c>
+      <c r="AP39">
+        <v>2.799998426437384</v>
+      </c>
       <c r="AQ39">
         <v>2.925002336502075</v>
       </c>
@@ -18841,6 +18850,9 @@
       <c r="AO40">
         <v>1.824998903274533</v>
       </c>
+      <c r="AP40">
+        <v>2.825001049041759</v>
+      </c>
       <c r="AQ40">
         <v>2.974998998641965</v>
       </c>
@@ -18969,6 +18981,9 @@
       <c r="AO41">
         <v>1.750002813339236</v>
       </c>
+      <c r="AP41">
+        <v>2.724999761581429</v>
+      </c>
       <c r="AQ41">
         <v>3.075002145767215</v>
       </c>
@@ -19097,6 +19112,9 @@
       <c r="AO42">
         <v>1.975002861022944</v>
       </c>
+      <c r="AP42">
+        <v>2.62500185966492</v>
+      </c>
       <c r="AQ42">
         <v>2.725002145767206</v>
       </c>
@@ -19225,6 +19243,9 @@
       <c r="AO43">
         <v>2.149998521804804</v>
       </c>
+      <c r="AP43">
+        <v>2.174997472763067</v>
+      </c>
       <c r="AQ43">
         <v>2.200000858306879</v>
       </c>
@@ -19353,6 +19374,9 @@
       <c r="AO44">
         <v>1.524998283386225</v>
       </c>
+      <c r="AP44">
+        <v>1.699997758865351</v>
+      </c>
       <c r="AQ44">
         <v>1.725001668930048</v>
       </c>
@@ -19481,6 +19505,9 @@
       <c r="AO45">
         <v>1.22499756813049</v>
       </c>
+      <c r="AP45">
+        <v>1.325000381469735</v>
+      </c>
       <c r="AQ45">
         <v>1.22499756813049</v>
       </c>
@@ -19609,6 +19636,9 @@
       <c r="AO46">
         <v>0.4749991416931039</v>
       </c>
+      <c r="AP46">
+        <v>0.57499809265137</v>
+      </c>
       <c r="AQ46">
         <v>0.4749991416931039</v>
       </c>
@@ -19736,6 +19766,9 @@
       </c>
       <c r="AO47">
         <v>0.04999814033507732</v>
+      </c>
+      <c r="AP47">
+        <v>-2.384185791015625E-06</v>
       </c>
       <c r="AQ47">
         <v>1.764297479667221E-06</v>
@@ -20148,49 +20181,49 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C5">
         <v>0.04303097099143827</v>
       </c>
       <c r="D5">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E5">
         <v>0.05930303901511991</v>
       </c>
       <c r="F5">
-        <v>0.02237796157676541</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G5">
         <v>0.05523800224143827</v>
       </c>
       <c r="H5">
-        <v>0.024413460195845</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="I5">
         <v>0.05116700500327909</v>
       </c>
       <c r="J5">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="K5">
         <v>0.04303097099143827</v>
       </c>
       <c r="L5">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="M5">
         <v>0.04709600776511991</v>
       </c>
       <c r="N5">
-        <v>0.02237796157676541</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O5">
         <v>0.05523800224143827</v>
       </c>
       <c r="P5">
-        <v>0.024413460195845</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="Q5">
         <v>0.05116700500327909</v>
@@ -20220,13 +20253,13 @@
         <v>0.05523800224143827</v>
       </c>
       <c r="Z5">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AA5">
         <v>0.06337403625327909</v>
       </c>
       <c r="AB5">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC5">
         <v>0.06337403625327909</v>
@@ -20279,49 +20312,49 @@
         <v>0.1</v>
       </c>
       <c r="B6">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C6">
         <v>0.05116700500327909</v>
       </c>
       <c r="D6">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="E6">
         <v>0.05116700500327909</v>
       </c>
       <c r="F6">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="G6">
         <v>0.06744503349143828</v>
       </c>
       <c r="H6">
-        <v>0.01007556289512479</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="I6">
         <v>0.06337403625327909</v>
       </c>
       <c r="J6">
-        <v>0.02930104106742704</v>
+        <v>0.04303097099143827</v>
       </c>
       <c r="K6">
         <v>0.04303097099143827</v>
       </c>
       <c r="L6">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="M6">
         <v>0.05116700500327909</v>
       </c>
       <c r="N6">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="O6">
         <v>0.06744503349143828</v>
       </c>
       <c r="P6">
-        <v>0.01007556289512479</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="Q6">
         <v>0.06337403625327909</v>
@@ -20351,13 +20384,13 @@
         <v>0.05930303901511991</v>
       </c>
       <c r="Z6">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA6">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB6">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC6">
         <v>0.06337403625327909</v>
@@ -20410,49 +20443,49 @@
         <v>0.2</v>
       </c>
       <c r="B7">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C7">
         <v>0.05523800224143827</v>
       </c>
       <c r="D7">
-        <v>0.01617907852012479</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="E7">
         <v>0.06337403625327909</v>
       </c>
       <c r="F7">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="G7">
         <v>0.04709600776511991</v>
       </c>
       <c r="H7">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="I7">
         <v>0.06744503349143828</v>
       </c>
       <c r="J7">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K7">
         <v>0.04303097099143827</v>
       </c>
       <c r="L7">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="M7">
         <v>0.05116700500327909</v>
       </c>
       <c r="N7">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="O7">
         <v>0.04709600776511991</v>
       </c>
       <c r="P7">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="Q7">
         <v>0.06744503349143828</v>
@@ -20482,13 +20515,13 @@
         <v>0.05523800224143827</v>
       </c>
       <c r="Z7">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA7">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB7">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC7">
         <v>0.05930303901511991</v>
@@ -20541,49 +20574,49 @@
         <v>0.3</v>
       </c>
       <c r="B8">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C8">
         <v>0.05930303901511991</v>
       </c>
       <c r="D8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E8">
         <v>0.06337403625327909</v>
       </c>
       <c r="F8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G8">
         <v>0.05930303901511991</v>
       </c>
       <c r="H8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I8">
         <v>0.08371710151511991</v>
       </c>
       <c r="J8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K8">
         <v>0.04709600776511991</v>
       </c>
       <c r="L8">
-        <v>0.01769899696189725</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M8">
         <v>0.06744503349143828</v>
       </c>
       <c r="N8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O8">
         <v>0.05930303901511991</v>
       </c>
       <c r="P8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q8">
         <v>0.08371710151511991</v>
@@ -20613,13 +20646,13 @@
         <v>0.05523800224143827</v>
       </c>
       <c r="Z8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA8">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB8">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC8">
         <v>0.05116700500327909</v>
@@ -20672,49 +20705,49 @@
         <v>0.4</v>
       </c>
       <c r="B9">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="C9">
         <v>0.05523800224143827</v>
       </c>
       <c r="D9">
-        <v>0.02878844112235868</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="E9">
         <v>0.05930303901511991</v>
       </c>
       <c r="F9">
-        <v>0.0247174438841995</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G9">
         <v>0.05523800224143827</v>
       </c>
       <c r="H9">
-        <v>0.02146601051170194</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="I9">
         <v>0.05930303901511991</v>
       </c>
       <c r="J9">
-        <v>0.01617907852012479</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="K9">
         <v>0.04709600776511991</v>
       </c>
       <c r="L9">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="M9">
         <v>0.05930303901511991</v>
       </c>
       <c r="N9">
-        <v>0.0247174438841995</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O9">
         <v>0.05523800224143827</v>
       </c>
       <c r="P9">
-        <v>0.02146601051170194</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="Q9">
         <v>0.05930303901511991</v>
@@ -20744,13 +20777,13 @@
         <v>0.05523800224143827</v>
       </c>
       <c r="Z9">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AA9">
         <v>0.05930303901511991</v>
       </c>
       <c r="AB9">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC9">
         <v>0.05116700500327909</v>
@@ -20803,49 +20836,49 @@
         <v>0.5</v>
       </c>
       <c r="B10">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C10">
         <v>0.05116700500327909</v>
       </c>
       <c r="D10">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E10">
         <v>0.07965206474143828</v>
       </c>
       <c r="F10">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G10">
         <v>0.07558106750327909</v>
       </c>
       <c r="H10">
-        <v>0.0205510792143997</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="I10">
         <v>0.06744503349143828</v>
       </c>
       <c r="J10">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K10">
         <v>0.04303097099143827</v>
       </c>
       <c r="L10">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M10">
         <v>0.03488897651511991</v>
       </c>
       <c r="N10">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O10">
         <v>0.07558106750327909</v>
       </c>
       <c r="P10">
-        <v>0.0205510792143997</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="Q10">
         <v>0.06744503349143828</v>
@@ -20875,13 +20908,13 @@
         <v>0.05116700500327909</v>
       </c>
       <c r="Z10">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AA10">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB10">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC10">
         <v>0.05523800224143827</v>
@@ -20934,49 +20967,49 @@
         <v>0.6</v>
       </c>
       <c r="B11">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="C11">
         <v>0.04709600776511991</v>
       </c>
       <c r="D11">
-        <v>0.024413460195845</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="E11">
         <v>0.05523800224143827</v>
       </c>
       <c r="F11">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G11">
         <v>0.05930303901511991</v>
       </c>
       <c r="H11">
-        <v>0.02146601051170194</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="I11">
         <v>0.06744503349143828</v>
       </c>
       <c r="J11">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="K11">
         <v>0.05116700500327909</v>
       </c>
       <c r="L11">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M11">
         <v>0.04709600776511991</v>
       </c>
       <c r="N11">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O11">
         <v>0.05930303901511991</v>
       </c>
       <c r="P11">
-        <v>0.02146601051170194</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="Q11">
         <v>0.06744503349143828</v>
@@ -21006,13 +21039,13 @@
         <v>0.05116700500327909</v>
       </c>
       <c r="Z11">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA11">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB11">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC11">
         <v>0.05930303901511991</v>
@@ -21065,49 +21098,49 @@
         <v>0.7</v>
       </c>
       <c r="B12">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C12">
         <v>0.05523800224143827</v>
       </c>
       <c r="D12">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E12">
         <v>0.04709600776511991</v>
       </c>
       <c r="F12">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G12">
         <v>0.05523800224143827</v>
       </c>
       <c r="H12">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="I12">
         <v>0.04303097099143827</v>
       </c>
       <c r="J12">
-        <v>0.01536249488670194</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K12">
         <v>0.04303097099143827</v>
       </c>
       <c r="L12">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M12">
         <v>0.05930303901511991</v>
       </c>
       <c r="N12">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O12">
         <v>0.05523800224143827</v>
       </c>
       <c r="P12">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="Q12">
         <v>0.04303097099143827</v>
@@ -21137,13 +21170,13 @@
         <v>0.05116700500327909</v>
       </c>
       <c r="Z12">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AA12">
         <v>0.05116700500327909</v>
       </c>
       <c r="AB12">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC12">
         <v>0.05116700500327909</v>
@@ -21196,49 +21229,49 @@
         <v>0.8</v>
       </c>
       <c r="B13">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C13">
         <v>0.05523800224143827</v>
       </c>
       <c r="D13">
-        <v>0.01505851119834745</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="E13">
         <v>0.03895997375327909</v>
       </c>
       <c r="F13">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G13">
         <v>0.04303097099143827</v>
       </c>
       <c r="H13">
-        <v>0.02228259414512479</v>
+        <v>0.04303097099143827</v>
       </c>
       <c r="I13">
         <v>0.05523800224143827</v>
       </c>
       <c r="J13">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K13">
         <v>0.04709600776511991</v>
       </c>
       <c r="L13">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M13">
         <v>0.05523800224143827</v>
       </c>
       <c r="N13">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O13">
         <v>0.04303097099143827</v>
       </c>
       <c r="P13">
-        <v>0.02228259414512479</v>
+        <v>0.04303097099143827</v>
       </c>
       <c r="Q13">
         <v>0.05523800224143827</v>
@@ -21268,13 +21301,13 @@
         <v>0.08778809875327909</v>
       </c>
       <c r="Z13">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA13">
         <v>0.05930303901511991</v>
       </c>
       <c r="AB13">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AC13">
         <v>0.07558106750327909</v>
@@ -21327,49 +21360,49 @@
         <v>0.9</v>
       </c>
       <c r="B14">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C14">
         <v>0.04709600776511991</v>
       </c>
       <c r="D14">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E14">
         <v>0.04709600776511991</v>
       </c>
       <c r="F14">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G14">
         <v>0.04709600776511991</v>
       </c>
       <c r="H14">
-        <v>0.02319752544242704</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="I14">
         <v>0.05930303901511991</v>
       </c>
       <c r="J14">
-        <v>0.02939640849906766</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K14">
         <v>0.05523800224143827</v>
       </c>
       <c r="L14">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="M14">
         <v>0.05930303901511991</v>
       </c>
       <c r="N14">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O14">
         <v>0.04709600776511991</v>
       </c>
       <c r="P14">
-        <v>0.02319752544242704</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="Q14">
         <v>0.05930303901511991</v>
@@ -21399,13 +21432,13 @@
         <v>0.08778809875327909</v>
       </c>
       <c r="Z14">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AA14">
         <v>0.06744503349143828</v>
       </c>
       <c r="AB14">
-        <v>0.01648306220847928</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AC14">
         <v>0.07558106750327909</v>
@@ -21883,121 +21916,121 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C21">
         <v>0.05116700500327909</v>
       </c>
       <c r="D21">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="E21">
         <v>0.05116700500327909</v>
       </c>
       <c r="F21">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="G21">
         <v>0.04709600776511991</v>
       </c>
       <c r="H21">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I21">
         <v>0.03895997375327909</v>
       </c>
       <c r="J21">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K21">
         <v>0.05523800224143827</v>
       </c>
       <c r="L21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="M21">
         <v>0.01861690849143827</v>
       </c>
       <c r="N21">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="O21">
         <v>0.04709600776511991</v>
       </c>
       <c r="P21">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q21">
         <v>0.03895997375327909</v>
       </c>
       <c r="R21">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="S21">
         <v>0.04303097099143827</v>
       </c>
       <c r="T21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="U21">
         <v>0.03895997375327909</v>
       </c>
       <c r="V21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="W21">
         <v>0.03488897651511991</v>
       </c>
       <c r="X21">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Y21">
         <v>0.03082393974143827</v>
       </c>
       <c r="Z21">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AA21">
         <v>0.04303097099143827</v>
       </c>
       <c r="AB21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AC21">
         <v>0.03895997375327909</v>
       </c>
       <c r="AD21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AE21">
         <v>0.03488897651511991</v>
       </c>
       <c r="AF21">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AG21">
         <v>0.03082393974143827</v>
       </c>
       <c r="AH21">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AI21">
         <v>0.04709600776511991</v>
       </c>
       <c r="AJ21">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AK21">
         <v>0.01861690849143827</v>
       </c>
       <c r="AL21">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AM21">
         <v>0.05930303901511991</v>
       </c>
       <c r="AN21">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AO21">
         <v>0.01047491401511991</v>
@@ -22014,121 +22047,121 @@
         <v>0.1</v>
       </c>
       <c r="B22">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C22">
         <v>0.04303097099143827</v>
       </c>
       <c r="D22">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E22">
         <v>0.04303097099143827</v>
       </c>
       <c r="F22">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G22">
         <v>0.04709600776511991</v>
       </c>
       <c r="H22">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I22">
         <v>0.04709600776511991</v>
       </c>
       <c r="J22">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="K22">
         <v>0.04303097099143827</v>
       </c>
       <c r="L22">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="M22">
         <v>0.03488897651511991</v>
       </c>
       <c r="N22">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O22">
         <v>0.04709600776511991</v>
       </c>
       <c r="P22">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q22">
         <v>0.04709600776511991</v>
       </c>
       <c r="R22">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="S22">
         <v>0.03488897651511991</v>
       </c>
       <c r="T22">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="U22">
         <v>0.03895997375327909</v>
       </c>
       <c r="V22">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="W22">
         <v>0.03488897651511991</v>
       </c>
       <c r="X22">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Y22">
         <v>0.03082393974143827</v>
       </c>
       <c r="Z22">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AA22">
         <v>0.03488897651511991</v>
       </c>
       <c r="AB22">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AC22">
         <v>0.03895997375327909</v>
       </c>
       <c r="AD22">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AE22">
         <v>0.03488897651511991</v>
       </c>
       <c r="AF22">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AG22">
         <v>0.03082393974143827</v>
       </c>
       <c r="AH22">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AI22">
         <v>0.04303097099143827</v>
       </c>
       <c r="AJ22">
-        <v>0.01007556289512479</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AK22">
         <v>0.03895997375327909</v>
       </c>
       <c r="AL22">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AM22">
         <v>0.03488897651511991</v>
       </c>
       <c r="AN22">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AO22">
         <v>0.02268194526511991</v>
@@ -22145,121 +22178,121 @@
         <v>0.2</v>
       </c>
       <c r="B23">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C23">
         <v>0.04709600776511991</v>
       </c>
       <c r="D23">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="E23">
         <v>0.02268194526511991</v>
       </c>
       <c r="F23">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G23">
         <v>0.03488897651511991</v>
       </c>
       <c r="H23">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I23">
         <v>0.01047491401511991</v>
       </c>
       <c r="J23">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="K23">
         <v>0.04709600776511991</v>
       </c>
       <c r="L23">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="M23">
         <v>0.04709600776511991</v>
       </c>
       <c r="N23">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O23">
         <v>0.03488897651511991</v>
       </c>
       <c r="P23">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q23">
         <v>0.01047491401511991</v>
       </c>
       <c r="R23">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="S23">
         <v>0.03895997375327909</v>
       </c>
       <c r="T23">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="U23">
         <v>0.03488897651511991</v>
       </c>
       <c r="V23">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="W23">
         <v>0.03082393974143827</v>
       </c>
       <c r="X23">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="Y23">
         <v>0.02268194526511991</v>
       </c>
       <c r="Z23">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AA23">
         <v>0.03895997375327909</v>
       </c>
       <c r="AB23">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AC23">
         <v>0.03488897651511991</v>
       </c>
       <c r="AD23">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AE23">
         <v>0.02675294250327909</v>
       </c>
       <c r="AF23">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AG23">
         <v>0.02268194526511991</v>
       </c>
       <c r="AH23">
-        <v>0.01943349212486112</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AI23">
         <v>0.03488897651511991</v>
       </c>
       <c r="AJ23">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AK23">
         <v>0.03488897651511991</v>
       </c>
       <c r="AL23">
-        <v>0.02116202682334745</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AM23">
         <v>0.05116700500327909</v>
       </c>
       <c r="AN23">
-        <v>0.01912652820426786</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AO23">
         <v>0.02675294250327909</v>
@@ -22276,121 +22309,121 @@
         <v>0.3</v>
       </c>
       <c r="B24">
-        <v>0.01821159690696561</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="C24">
         <v>0.03895997375327909</v>
       </c>
       <c r="D24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="E24">
         <v>0.04709600776511991</v>
       </c>
       <c r="F24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="G24">
         <v>0.04709600776511991</v>
       </c>
       <c r="H24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="I24">
         <v>0.03895997375327909</v>
       </c>
       <c r="J24">
-        <v>0.0141435799010452</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="K24">
         <v>0.03895997375327909</v>
       </c>
       <c r="L24">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="M24">
         <v>0.05523800224143827</v>
       </c>
       <c r="N24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="O24">
         <v>0.04709600776511991</v>
       </c>
       <c r="P24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="Q24">
         <v>0.03895997375327909</v>
       </c>
       <c r="R24">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="S24">
         <v>0.03895997375327909</v>
       </c>
       <c r="T24">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="U24">
         <v>0.03895997375327909</v>
       </c>
       <c r="V24">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="W24">
         <v>0.03488897651511991</v>
       </c>
       <c r="X24">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="Y24">
         <v>0.03082393974143827</v>
       </c>
       <c r="Z24">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AA24">
         <v>0.03895997375327909</v>
       </c>
       <c r="AB24">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AC24">
         <v>0.03895997375327909</v>
       </c>
       <c r="AD24">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AE24">
         <v>0.03488897651511991</v>
       </c>
       <c r="AF24">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AG24">
         <v>0.03082393974143827</v>
       </c>
       <c r="AH24">
-        <v>0.02116202682334745</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AI24">
         <v>0.03895997375327909</v>
       </c>
       <c r="AJ24">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AK24">
         <v>0.03488897651511991</v>
       </c>
       <c r="AL24">
-        <v>0.01648306220847928</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AM24">
         <v>0.03488897651511991</v>
       </c>
       <c r="AN24">
-        <v>0.02350150913078153</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AO24">
         <v>0.02268194526511991</v>
@@ -22407,121 +22440,121 @@
         <v>0.4</v>
       </c>
       <c r="B25">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C25">
         <v>0.04303097099143827</v>
       </c>
       <c r="D25">
-        <v>0.01769899696189725</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E25">
         <v>0.04303097099143827</v>
       </c>
       <c r="F25">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="G25">
         <v>0.03895997375327909</v>
       </c>
       <c r="H25">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I25">
         <v>0.03895997375327909</v>
       </c>
       <c r="J25">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K25">
         <v>0.04709600776511991</v>
       </c>
       <c r="L25">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M25">
         <v>0.04303097099143827</v>
       </c>
       <c r="N25">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="O25">
         <v>0.03895997375327909</v>
       </c>
       <c r="P25">
-        <v>0.008344047964399692</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q25">
         <v>0.03895997375327909</v>
       </c>
       <c r="R25">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="S25">
         <v>0.04303097099143827</v>
       </c>
       <c r="T25">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="U25">
         <v>0.03895997375327909</v>
       </c>
       <c r="V25">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="W25">
         <v>0.03488897651511991</v>
       </c>
       <c r="X25">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="Y25">
         <v>0.03895997375327909</v>
       </c>
       <c r="Z25">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AA25">
         <v>0.04303097099143827</v>
       </c>
       <c r="AB25">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AC25">
         <v>0.03895997375327909</v>
       </c>
       <c r="AD25">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AE25">
         <v>0.03488897651511991</v>
       </c>
       <c r="AF25">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AG25">
         <v>0.03895997375327909</v>
       </c>
       <c r="AH25">
-        <v>0.01007556289512479</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AI25">
         <v>0.04303097099143827</v>
       </c>
       <c r="AJ25">
-        <v>0.02207397788841092</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AK25">
         <v>0.03895997375327909</v>
       </c>
       <c r="AL25">
-        <v>0.01739799350578153</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AM25">
         <v>0.03082393974143827</v>
       </c>
       <c r="AN25">
-        <v>0.01007556289512479</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AO25">
         <v>0.04303097099143827</v>
@@ -22538,121 +22571,121 @@
         <v>0.5</v>
       </c>
       <c r="B26">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="C26">
         <v>0.04303097099143827</v>
       </c>
       <c r="D26">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="E26">
         <v>0.04303097099143827</v>
       </c>
       <c r="F26">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="G26">
         <v>0.03082393974143827</v>
       </c>
       <c r="H26">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I26">
         <v>0.05523800224143827</v>
       </c>
       <c r="J26">
-        <v>0.01505851119834745</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="K26">
         <v>0.04303097099143827</v>
       </c>
       <c r="L26">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M26">
         <v>0.05930303901511991</v>
       </c>
       <c r="N26">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="O26">
         <v>0.03082393974143827</v>
       </c>
       <c r="P26">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q26">
         <v>0.05523800224143827</v>
       </c>
       <c r="R26">
-        <v>0.01912652820426786</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="S26">
         <v>0.04303097099143827</v>
       </c>
       <c r="T26">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="U26">
         <v>0.04709600776511991</v>
       </c>
       <c r="V26">
-        <v>0.0205510792143997</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="W26">
         <v>0.04709600776511991</v>
       </c>
       <c r="X26">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="Y26">
         <v>0.05116700500327909</v>
       </c>
       <c r="Z26">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AA26">
         <v>0.04303097099143827</v>
       </c>
       <c r="AB26">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AC26">
         <v>0.05116700500327909</v>
       </c>
       <c r="AD26">
-        <v>0.0205510792143997</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="AE26">
         <v>0.04709600776511991</v>
       </c>
       <c r="AF26">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AG26">
         <v>0.05116700500327909</v>
       </c>
       <c r="AH26">
-        <v>0.03834902614433134</v>
+        <v>0.04709600776511991</v>
       </c>
       <c r="AI26">
         <v>0.05116700500327909</v>
       </c>
       <c r="AJ26">
-        <v>0.01444756358939969</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AK26">
         <v>0.04709600776511991</v>
       </c>
       <c r="AL26">
-        <v>0.0205510792143997</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="AM26">
         <v>0.04709600776511991</v>
       </c>
       <c r="AN26">
-        <v>0.01851856082755888</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AO26">
         <v>0.05523800224143827</v>
@@ -22669,121 +22702,121 @@
         <v>0.6</v>
       </c>
       <c r="B27">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="C27">
         <v>0.04303097099143827</v>
       </c>
       <c r="D27">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E27">
         <v>0.04303097099143827</v>
       </c>
       <c r="F27">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G27">
         <v>0.04303097099143827</v>
       </c>
       <c r="H27">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="I27">
         <v>0.04303097099143827</v>
       </c>
       <c r="J27">
-        <v>0.01821159690696561</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="K27">
         <v>0.05523800224143827</v>
       </c>
       <c r="L27">
-        <v>0.01241504520255887</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="M27">
         <v>0.04709600776511991</v>
       </c>
       <c r="N27">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O27">
         <v>0.04303097099143827</v>
       </c>
       <c r="P27">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="Q27">
         <v>0.04303097099143827</v>
       </c>
       <c r="R27">
-        <v>0.02848147720176541</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="S27">
         <v>0.04709600776511991</v>
       </c>
       <c r="T27">
-        <v>0.02116202682334745</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="U27">
         <v>0.05116700500327909</v>
       </c>
       <c r="V27">
-        <v>0.02085804313499295</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="W27">
         <v>0.04709600776511991</v>
       </c>
       <c r="X27">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="Y27">
         <v>0.05523800224143827</v>
       </c>
       <c r="Z27">
-        <v>0.02848147720176541</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AA27">
         <v>0.04709600776511991</v>
       </c>
       <c r="AB27">
-        <v>0.02116202682334745</v>
+        <v>0.02675294250327909</v>
       </c>
       <c r="AC27">
         <v>0.05116700500327909</v>
       </c>
       <c r="AD27">
-        <v>0.02085804313499295</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AE27">
         <v>0.05116700500327909</v>
       </c>
       <c r="AF27">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AG27">
         <v>0.05523800224143827</v>
       </c>
       <c r="AH27">
-        <v>0.01943349212486112</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AI27">
         <v>0.04709600776511991</v>
       </c>
       <c r="AJ27">
-        <v>0.03164052337486112</v>
+        <v>0.04303097099143827</v>
       </c>
       <c r="AK27">
         <v>0.05930303901511991</v>
       </c>
       <c r="AL27">
-        <v>0.02756952613670194</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="AM27">
         <v>0.05116700500327909</v>
       </c>
       <c r="AN27">
-        <v>0.02553700774986112</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AO27">
         <v>0.04303097099143827</v>
@@ -22800,121 +22833,121 @@
         <v>0.7</v>
       </c>
       <c r="B28">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="C28">
         <v>0.04303097099143827</v>
       </c>
       <c r="D28">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E28">
         <v>0.04303097099143827</v>
       </c>
       <c r="F28">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="G28">
         <v>0.04303097099143827</v>
       </c>
       <c r="H28">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I28">
         <v>0.05116700500327909</v>
       </c>
       <c r="J28">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K28">
         <v>0.05116700500327909</v>
       </c>
       <c r="L28">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M28">
         <v>0.05523800224143827</v>
       </c>
       <c r="N28">
-        <v>0.01210808128196561</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="O28">
         <v>0.04303097099143827</v>
       </c>
       <c r="P28">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q28">
         <v>0.05116700500327909</v>
       </c>
       <c r="R28">
-        <v>0.02410947650749052</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="S28">
         <v>0.04303097099143827</v>
       </c>
       <c r="T28">
-        <v>0.01943349212486112</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="U28">
         <v>0.05930303901511991</v>
       </c>
       <c r="V28">
-        <v>0.02289056152183378</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="W28">
         <v>0.05116700500327909</v>
       </c>
       <c r="X28">
-        <v>0.03479360908347928</v>
+        <v>0.06337403625327909</v>
       </c>
       <c r="Y28">
         <v>0.06744503349143828</v>
       </c>
       <c r="Z28">
-        <v>0.02410947650749052</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AA28">
         <v>0.03895997375327909</v>
       </c>
       <c r="AB28">
-        <v>0.01709400981742704</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AC28">
         <v>0.05930303901511991</v>
       </c>
       <c r="AD28">
-        <v>0.02289056152183378</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="AE28">
         <v>0.05116700500327909</v>
       </c>
       <c r="AF28">
-        <v>0.03479360908347928</v>
+        <v>0.06337403625327909</v>
       </c>
       <c r="AG28">
         <v>0.06744503349143828</v>
       </c>
       <c r="AH28">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AI28">
         <v>0.05116700500327909</v>
       </c>
       <c r="AJ28">
-        <v>0.03255247443992459</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AK28">
         <v>0.04303097099143827</v>
       </c>
       <c r="AL28">
-        <v>0.02319752544242704</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AM28">
         <v>0.05523800224143827</v>
       </c>
       <c r="AN28">
-        <v>0.02380251258689725</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AO28">
         <v>0.05116700500327909</v>
@@ -22931,121 +22964,121 @@
         <v>0.8</v>
       </c>
       <c r="B29">
-        <v>0.01037954658347928</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C29">
         <v>0.03895997375327909</v>
       </c>
       <c r="D29">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="E29">
         <v>0.03895997375327909</v>
       </c>
       <c r="F29">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G29">
         <v>0.03895997375327909</v>
       </c>
       <c r="H29">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="I29">
         <v>0.05116700500327909</v>
       </c>
       <c r="J29">
-        <v>0.0080400642760452</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="K29">
         <v>0.04303097099143827</v>
       </c>
       <c r="L29">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M29">
         <v>0.04303097099143827</v>
       </c>
       <c r="N29">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O29">
         <v>0.03895997375327909</v>
       </c>
       <c r="P29">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="Q29">
         <v>0.05116700500327909</v>
       </c>
       <c r="R29">
-        <v>0.02614199489433134</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="S29">
         <v>0.05523800224143827</v>
       </c>
       <c r="T29">
-        <v>0.02410947650749052</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="U29">
         <v>0.07965206474143828</v>
       </c>
       <c r="V29">
-        <v>0.04506348937827909</v>
+        <v>0.05116700500327909</v>
       </c>
       <c r="W29">
         <v>0.07151007026511991</v>
       </c>
       <c r="X29">
-        <v>0.04709898799735868</v>
+        <v>0.05523800224143827</v>
       </c>
       <c r="Y29">
         <v>0.08371710151511991</v>
       </c>
       <c r="Z29">
-        <v>0.02614199489433134</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AA29">
         <v>0.05523800224143827</v>
       </c>
       <c r="AB29">
-        <v>0.02410947650749052</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AC29">
         <v>0.07965206474143828</v>
       </c>
       <c r="AD29">
-        <v>0.04506348937827909</v>
+        <v>0.05116700500327909</v>
       </c>
       <c r="AE29">
         <v>0.07151007026511991</v>
       </c>
       <c r="AF29">
-        <v>0.04709898799735868</v>
+        <v>0.05523800224143827</v>
       </c>
       <c r="AG29">
         <v>0.07965206474143828</v>
       </c>
       <c r="AH29">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AI29">
         <v>0.05930303901511991</v>
       </c>
       <c r="AJ29">
-        <v>0.0247174438841995</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AK29">
         <v>0.05116700500327909</v>
       </c>
       <c r="AL29">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AM29">
         <v>0.05523800224143827</v>
       </c>
       <c r="AN29">
-        <v>0.02176999420005643</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="AO29">
         <v>0.05116700500327909</v>
@@ -23062,121 +23095,121 @@
         <v>0.9</v>
       </c>
       <c r="B30">
-        <v>0.01271902889091336</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="C30">
         <v>0.04303097099143827</v>
       </c>
       <c r="D30">
-        <v>0.01678704589683377</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="E30">
         <v>0.05116700500327909</v>
       </c>
       <c r="F30">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="G30">
         <v>0.03488897651511991</v>
       </c>
       <c r="H30">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="I30">
         <v>0.05523800224143827</v>
       </c>
       <c r="J30">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="K30">
         <v>0.04303097099143827</v>
       </c>
       <c r="L30">
-        <v>0.00600456565696561</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="M30">
         <v>0.05116700500327909</v>
       </c>
       <c r="N30">
-        <v>0.01068353027183377</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="O30">
         <v>0.03488897651511991</v>
       </c>
       <c r="P30">
-        <v>0.01475452750999296</v>
+        <v>0.01861690849143827</v>
       </c>
       <c r="Q30">
         <v>0.05523800224143827</v>
       </c>
       <c r="R30">
-        <v>0.04333495467979276</v>
+        <v>0.04303097099143827</v>
       </c>
       <c r="S30">
         <v>0.05930303901511991</v>
       </c>
       <c r="T30">
-        <v>0.04363893836814725</v>
+        <v>0.03895997375327909</v>
       </c>
       <c r="U30">
         <v>0.08778809875327909</v>
       </c>
       <c r="V30">
-        <v>0.04943847030479276</v>
+        <v>0.05523800224143827</v>
       </c>
       <c r="W30">
         <v>0.07558106750327909</v>
       </c>
       <c r="X30">
-        <v>0.05554198592979277</v>
+        <v>0.06744503349143828</v>
       </c>
       <c r="Y30">
         <v>0.07965206474143828</v>
       </c>
       <c r="Z30">
-        <v>0.03723143905479276</v>
+        <v>0.03082393974143827</v>
       </c>
       <c r="AA30">
         <v>0.05930303901511991</v>
       </c>
       <c r="AB30">
-        <v>0.03926395744163358</v>
+        <v>0.03488897651511991</v>
       </c>
       <c r="AC30">
         <v>0.08778809875327909</v>
       </c>
       <c r="AD30">
-        <v>0.04943847030479276</v>
+        <v>0.05523800224143827</v>
       </c>
       <c r="AE30">
         <v>0.08371710151511991</v>
       </c>
       <c r="AF30">
-        <v>0.05554198592979277</v>
+        <v>0.06744503349143828</v>
       </c>
       <c r="AG30">
         <v>0.07965206474143828</v>
       </c>
       <c r="AH30">
-        <v>0.01302301257926786</v>
+        <v>0.01047491401511991</v>
       </c>
       <c r="AI30">
         <v>0.05930303901511991</v>
       </c>
       <c r="AJ30">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AK30">
         <v>0.06744503349143828</v>
       </c>
       <c r="AL30">
-        <v>0.01973449558097684</v>
+        <v>0.01454591125327909</v>
       </c>
       <c r="AM30">
         <v>0.05523800224143827</v>
       </c>
       <c r="AN30">
-        <v>0.02380251258689725</v>
+        <v>0.02268194526511991</v>
       </c>
       <c r="AO30">
         <v>0.05116700500327909</v>

</xml_diff>